<commit_message>
Update save_results_to_excel function to include ground truths and modify read_excel_file to return ground truths
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\coding\llm-fact-checker\llm-fact-checker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DCE128-757E-4F01-BCDA-A7B34A9C39D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650EE57B-011E-408F-99AD-689074378543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1395,15 +1395,15 @@
   <dimension ref="A1:C367"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B1" sqref="B1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="255.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="255.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1412,7 +1412,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1430,7 +1430,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>143</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>147</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>148</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>149</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>150</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>151</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>152</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>155</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>156</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>157</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>158</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>160</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>162</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>163</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>164</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>165</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>173</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>174</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>176</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>177</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>178</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>179</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>180</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>181</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>182</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>183</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>184</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>185</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>186</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>187</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>188</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>189</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>190</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>191</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>192</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>193</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>194</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>195</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>196</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>197</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>198</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>199</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>200</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>201</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="203" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>202</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>203</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>204</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>206</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>208</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>209</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>211</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>212</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>213</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>214</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>215</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>216</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>217</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="219" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>218</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>219</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="221" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>220</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="222" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>221</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>222</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="224" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>223</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="225" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>224</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="226" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>225</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="227" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>226</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="228" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>227</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="229" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>228</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="230" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>229</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="231" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>230</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="232" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>231</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>232</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="234" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>233</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>234</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>235</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="237" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>236</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="238" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>237</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>238</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>239</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>240</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>241</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>242</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="244" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>243</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="245" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>244</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="246" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>245</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>246</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="248" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>247</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="249" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>248</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="250" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>249</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="251" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>250</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="252" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>251</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="253" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>252</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="254" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>253</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>254</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="256" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>255</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>256</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="258" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>257</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="259" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>258</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="260" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>259</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="261" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>260</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="262" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>261</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="263" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>262</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="264" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>263</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="265" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>264</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="266" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>265</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="267" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>266</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="268" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>267</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="269" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>268</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="270" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>269</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="271" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>270</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="272" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>271</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="273" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>272</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="274" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>273</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="275" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>274</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="276" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>275</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="277" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>276</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="278" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>277</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="279" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>278</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="280" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>279</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="281" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>280</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="282" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>281</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="283" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>282</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="284" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>283</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="285" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>284</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="286" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>285</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="287" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>286</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="288" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>287</v>
       </c>
@@ -3711,7 +3711,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="289" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>288</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="290" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>289</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="291" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>290</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="292" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>291</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="293" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>292</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="294" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>293</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="295" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>294</v>
       </c>
@@ -3767,7 +3767,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="296" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>295</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="297" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>296</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="298" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>297</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="299" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>298</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="300" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>299</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="301" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>300</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="302" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>301</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="303" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>302</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="304" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>303</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="305" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>304</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="306" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>305</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="307" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>306</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="308" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>307</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="309" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>308</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="310" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>309</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="311" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>310</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="312" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>311</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="313" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>312</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="314" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>313</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="315" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>314</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="316" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>315</v>
       </c>
@@ -3935,7 +3935,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="317" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>316</v>
       </c>
@@ -3943,7 +3943,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="318" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>317</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="319" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>318</v>
       </c>
@@ -3959,7 +3959,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="320" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>319</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="321" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>320</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="322" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>321</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="323" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>322</v>
       </c>
@@ -3991,7 +3991,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="324" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>323</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="325" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>324</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="326" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>325</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="327" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>326</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="328" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>327</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="329" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>328</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="330" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>329</v>
       </c>
@@ -4047,7 +4047,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="331" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>330</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="332" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>331</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="333" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>332</v>
       </c>
@@ -4071,7 +4071,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="334" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>333</v>
       </c>
@@ -4079,7 +4079,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="335" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>334</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="336" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>335</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="337" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>336</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="338" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>337</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="339" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>338</v>
       </c>
@@ -4119,7 +4119,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="340" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>339</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="341" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>340</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="342" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>341</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="343" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>342</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="344" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>343</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="345" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>344</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="346" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>345</v>
       </c>
@@ -4175,7 +4175,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="347" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>346</v>
       </c>
@@ -4183,7 +4183,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="348" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>347</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="349" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>348</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="350" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>349</v>
       </c>
@@ -4207,7 +4207,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="351" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>350</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="352" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>351</v>
       </c>
@@ -4223,7 +4223,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="353" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>352</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="354" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>353</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="355" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>354</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="356" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>355</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="357" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>356</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="358" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>357</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="359" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>358</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="360" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>359</v>
       </c>
@@ -4287,7 +4287,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="361" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>360</v>
       </c>
@@ -4295,7 +4295,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="362" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>361</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="363" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>362</v>
       </c>
@@ -4311,7 +4311,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="364" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>363</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="365" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>364</v>
       </c>
@@ -4327,7 +4327,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="366" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>365</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="367" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>366</v>
       </c>

</xml_diff>